<commit_message>
10/01/24 commit - updated with end of season stats and info
</commit_message>
<xml_diff>
--- a/public/results/Bottoms Up 2024 League Stats - Week 11.xlsx
+++ b/public/results/Bottoms Up 2024 League Stats - Week 11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\CODE\golf-league-site\public\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480794D7-BC45-4456-87FC-D40954460A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0874025A-2118-42CF-82DB-C4743C5F222C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="615" yWindow="330" windowWidth="24330" windowHeight="13665" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1605" yWindow="600" windowWidth="22305" windowHeight="13695" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="14" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="126">
   <si>
     <t>Karen</t>
   </si>
@@ -431,6 +431,9 @@
   <si>
     <t>FIRST HALF (11 Rounds)</t>
   </si>
+  <si>
+    <t>= Under min # of rounds</t>
+  </si>
 </sst>
 </file>
 
@@ -571,7 +574,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -620,8 +623,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="52">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -1288,12 +1297,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="197">
+  <cellXfs count="209">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1688,6 +1721,19 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1695,11 +1741,65 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="15" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1734,88 +1834,6 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="15" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1831,12 +1849,80 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{FEB32575-F33B-455F-81F3-7FDBFE07DE6C}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF1A983"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF1A983"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1859,13 +1945,13 @@
       <sheetName val="Instructions"/>
       <sheetName val="Point System"/>
       <sheetName val="18-hole scores"/>
+      <sheetName val="9-hole scores"/>
       <sheetName val="Week 1"/>
       <sheetName val="Week 2"/>
-      <sheetName val="Week 3"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1">
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
         <row r="4">
           <cell r="A4">
             <v>-5</v>
@@ -1963,8 +2049,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
       <sheetData sheetId="4" refreshError="1"/>
       <sheetData sheetId="5" refreshError="1"/>
     </sheetDataSet>
@@ -2316,23 +2402,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="153" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="149"/>
-      <c r="J1" s="149"/>
-      <c r="K1" s="149"/>
-      <c r="L1" s="149"/>
-      <c r="M1" s="149"/>
-      <c r="N1" s="149"/>
-      <c r="O1" s="149"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="154"/>
+      <c r="O1" s="154"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -2346,23 +2432,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="155" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="149"/>
-      <c r="L2" s="149"/>
-      <c r="M2" s="149"/>
-      <c r="N2" s="149"/>
-      <c r="O2" s="149"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="154"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="154"/>
+      <c r="O2" s="154"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -3216,23 +3302,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="153" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="149"/>
-      <c r="J1" s="149"/>
-      <c r="K1" s="149"/>
-      <c r="L1" s="149"/>
-      <c r="M1" s="149"/>
-      <c r="N1" s="149"/>
-      <c r="O1" s="149"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="154"/>
+      <c r="O1" s="154"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -3246,23 +3332,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="155" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="149"/>
-      <c r="L2" s="149"/>
-      <c r="M2" s="149"/>
-      <c r="N2" s="149"/>
-      <c r="O2" s="149"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="154"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="154"/>
+      <c r="O2" s="154"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -4019,9 +4105,9 @@
       </c>
       <c r="O15" s="25"/>
       <c r="P15" s="46"/>
-      <c r="Q15" s="182"/>
-      <c r="R15" s="183"/>
-      <c r="S15" s="184"/>
+      <c r="Q15" s="194"/>
+      <c r="R15" s="195"/>
+      <c r="S15" s="196"/>
       <c r="T15" s="51">
         <v>35</v>
       </c>
@@ -4865,23 +4951,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="153" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="149"/>
-      <c r="J1" s="149"/>
-      <c r="K1" s="149"/>
-      <c r="L1" s="149"/>
-      <c r="M1" s="149"/>
-      <c r="N1" s="149"/>
-      <c r="O1" s="149"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="154"/>
+      <c r="O1" s="154"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -4895,23 +4981,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="155" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="149"/>
-      <c r="L2" s="149"/>
-      <c r="M2" s="149"/>
-      <c r="N2" s="149"/>
-      <c r="O2" s="149"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="154"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="154"/>
+      <c r="O2" s="154"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -6539,23 +6625,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="153" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="149"/>
-      <c r="J1" s="149"/>
-      <c r="K1" s="149"/>
-      <c r="L1" s="149"/>
-      <c r="M1" s="149"/>
-      <c r="N1" s="149"/>
-      <c r="O1" s="149"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="154"/>
+      <c r="O1" s="154"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -6569,23 +6655,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="155" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="149"/>
-      <c r="L2" s="149"/>
-      <c r="M2" s="149"/>
-      <c r="N2" s="149"/>
-      <c r="O2" s="149"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="154"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="154"/>
+      <c r="O2" s="154"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -7594,23 +7680,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="153" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="149"/>
-      <c r="J1" s="149"/>
-      <c r="K1" s="149"/>
-      <c r="L1" s="149"/>
-      <c r="M1" s="149"/>
-      <c r="N1" s="149"/>
-      <c r="O1" s="149"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="154"/>
+      <c r="O1" s="154"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -7624,23 +7710,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="155" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="149"/>
-      <c r="L2" s="149"/>
-      <c r="M2" s="149"/>
-      <c r="N2" s="149"/>
-      <c r="O2" s="149"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="154"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="154"/>
+      <c r="O2" s="154"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -8646,23 +8732,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="153" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="149"/>
-      <c r="J1" s="149"/>
-      <c r="K1" s="149"/>
-      <c r="L1" s="149"/>
-      <c r="M1" s="149"/>
-      <c r="N1" s="149"/>
-      <c r="O1" s="149"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="154"/>
+      <c r="O1" s="154"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -8676,23 +8762,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="155" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="149"/>
-      <c r="L2" s="149"/>
-      <c r="M2" s="149"/>
-      <c r="N2" s="149"/>
-      <c r="O2" s="149"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="154"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="154"/>
+      <c r="O2" s="154"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -10083,23 +10169,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="153" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="149"/>
-      <c r="J1" s="149"/>
-      <c r="K1" s="149"/>
-      <c r="L1" s="149"/>
-      <c r="M1" s="149"/>
-      <c r="N1" s="149"/>
-      <c r="O1" s="149"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="154"/>
+      <c r="O1" s="154"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -10113,23 +10199,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="155" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="149"/>
-      <c r="L2" s="149"/>
-      <c r="M2" s="149"/>
-      <c r="N2" s="149"/>
-      <c r="O2" s="149"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="154"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="154"/>
+      <c r="O2" s="154"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -11135,23 +11221,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="153" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="149"/>
-      <c r="J1" s="149"/>
-      <c r="K1" s="149"/>
-      <c r="L1" s="149"/>
-      <c r="M1" s="149"/>
-      <c r="N1" s="149"/>
-      <c r="O1" s="149"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="154"/>
+      <c r="O1" s="154"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -11165,23 +11251,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="155" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="149"/>
-      <c r="L2" s="149"/>
-      <c r="M2" s="149"/>
-      <c r="N2" s="149"/>
-      <c r="O2" s="149"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="154"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="154"/>
+      <c r="O2" s="154"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -12101,138 +12187,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" s="1" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="176" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="162" t="s">
+      <c r="B1" s="177"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="185" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="151" t="s">
+      <c r="E1" s="167" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="152"/>
-      <c r="G1" s="151" t="s">
+      <c r="F1" s="168"/>
+      <c r="G1" s="167" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="152"/>
-      <c r="I1" s="151" t="s">
+      <c r="H1" s="168"/>
+      <c r="I1" s="167" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="152"/>
-      <c r="K1" s="151" t="s">
+      <c r="J1" s="168"/>
+      <c r="K1" s="167" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="152"/>
-      <c r="M1" s="151" t="s">
+      <c r="L1" s="168"/>
+      <c r="M1" s="167" t="s">
         <v>87</v>
       </c>
-      <c r="N1" s="152"/>
-      <c r="O1" s="151" t="s">
+      <c r="N1" s="168"/>
+      <c r="O1" s="167" t="s">
         <v>101</v>
       </c>
-      <c r="P1" s="152"/>
-      <c r="Q1" s="151" t="s">
+      <c r="P1" s="168"/>
+      <c r="Q1" s="167" t="s">
         <v>106</v>
       </c>
-      <c r="R1" s="152"/>
-      <c r="S1" s="151" t="s">
+      <c r="R1" s="168"/>
+      <c r="S1" s="167" t="s">
         <v>110</v>
       </c>
-      <c r="T1" s="152"/>
-      <c r="U1" s="151" t="s">
+      <c r="T1" s="168"/>
+      <c r="U1" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="V1" s="152"/>
-      <c r="W1" s="151" t="s">
+      <c r="V1" s="168"/>
+      <c r="W1" s="167" t="s">
         <v>117</v>
       </c>
-      <c r="X1" s="152"/>
-      <c r="Y1" s="151" t="s">
+      <c r="X1" s="168"/>
+      <c r="Y1" s="167" t="s">
         <v>118</v>
       </c>
-      <c r="Z1" s="152"/>
-      <c r="AA1" s="171" t="s">
+      <c r="Z1" s="168"/>
+      <c r="AA1" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="AB1" s="167" t="s">
+      <c r="AB1" s="165" t="s">
         <v>105</v>
       </c>
-      <c r="AC1" s="175" t="s">
+      <c r="AC1" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="AD1" s="171" t="s">
+      <c r="AD1" s="169" t="s">
         <v>116</v>
       </c>
-      <c r="AE1" s="164" t="s">
+      <c r="AE1" s="162" t="s">
         <v>48</v>
       </c>
-      <c r="AF1" s="167" t="s">
+      <c r="AF1" s="165" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:32" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="155"/>
-      <c r="B2" s="156"/>
-      <c r="C2" s="160"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="169">
+      <c r="A2" s="178"/>
+      <c r="B2" s="179"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="159">
         <v>45418</v>
       </c>
-      <c r="F2" s="170"/>
-      <c r="G2" s="169">
+      <c r="F2" s="160"/>
+      <c r="G2" s="159">
         <v>45425</v>
       </c>
-      <c r="H2" s="170"/>
-      <c r="I2" s="169">
+      <c r="H2" s="160"/>
+      <c r="I2" s="159">
         <v>45432</v>
       </c>
-      <c r="J2" s="170"/>
-      <c r="K2" s="169">
+      <c r="J2" s="160"/>
+      <c r="K2" s="159">
         <v>45439</v>
       </c>
-      <c r="L2" s="170"/>
-      <c r="M2" s="169">
+      <c r="L2" s="160"/>
+      <c r="M2" s="159">
         <v>45446</v>
       </c>
-      <c r="N2" s="170"/>
-      <c r="O2" s="169">
+      <c r="N2" s="160"/>
+      <c r="O2" s="159">
         <v>45453</v>
       </c>
-      <c r="P2" s="170"/>
-      <c r="Q2" s="169">
+      <c r="P2" s="160"/>
+      <c r="Q2" s="159">
         <v>45460</v>
       </c>
-      <c r="R2" s="170"/>
-      <c r="S2" s="169">
+      <c r="R2" s="160"/>
+      <c r="S2" s="159">
         <v>45467</v>
       </c>
-      <c r="T2" s="170"/>
-      <c r="U2" s="169">
+      <c r="T2" s="160"/>
+      <c r="U2" s="159">
         <v>45474</v>
       </c>
-      <c r="V2" s="170"/>
-      <c r="W2" s="169">
+      <c r="V2" s="160"/>
+      <c r="W2" s="159">
         <v>45481</v>
       </c>
-      <c r="X2" s="170"/>
-      <c r="Y2" s="169">
+      <c r="X2" s="160"/>
+      <c r="Y2" s="159">
         <v>45488</v>
       </c>
-      <c r="Z2" s="170"/>
-      <c r="AA2" s="172"/>
-      <c r="AB2" s="168"/>
-      <c r="AC2" s="176"/>
-      <c r="AD2" s="172"/>
-      <c r="AE2" s="165"/>
-      <c r="AF2" s="168"/>
+      <c r="Z2" s="160"/>
+      <c r="AA2" s="170"/>
+      <c r="AB2" s="166"/>
+      <c r="AC2" s="174"/>
+      <c r="AD2" s="170"/>
+      <c r="AE2" s="163"/>
+      <c r="AF2" s="166"/>
     </row>
     <row r="3" spans="1:32" s="1" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="157"/>
-      <c r="B3" s="158"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="163"/>
+      <c r="A3" s="180"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="184"/>
+      <c r="D3" s="186"/>
       <c r="E3" s="61" t="s">
         <v>28</v>
       </c>
@@ -12299,12 +12385,12 @@
       <c r="Z3" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="AA3" s="173"/>
-      <c r="AB3" s="174"/>
-      <c r="AC3" s="177"/>
-      <c r="AD3" s="172"/>
-      <c r="AE3" s="166"/>
-      <c r="AF3" s="168"/>
+      <c r="AA3" s="171"/>
+      <c r="AB3" s="172"/>
+      <c r="AC3" s="175"/>
+      <c r="AD3" s="170"/>
+      <c r="AE3" s="164"/>
+      <c r="AF3" s="166"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
@@ -13821,50 +13907,50 @@
     <row r="25" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="59"/>
       <c r="C25" s="59"/>
-      <c r="F25" s="178" t="s">
+      <c r="F25" s="156" t="s">
         <v>30</v>
       </c>
-      <c r="G25" s="178"/>
+      <c r="G25" s="156"/>
       <c r="H25" s="128" t="s">
         <v>32</v>
       </c>
-      <c r="O25" s="179" t="s">
+      <c r="O25" s="157" t="s">
         <v>120</v>
       </c>
-      <c r="P25" s="179"/>
-      <c r="Q25" s="180" t="s">
+      <c r="P25" s="157"/>
+      <c r="Q25" s="161" t="s">
         <v>32</v>
       </c>
-      <c r="R25" s="180"/>
+      <c r="R25" s="161"/>
       <c r="AA25" s="127"/>
       <c r="AC25"/>
     </row>
     <row r="26" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="59"/>
       <c r="C26" s="59"/>
-      <c r="F26" s="178" t="s">
+      <c r="F26" s="156" t="s">
         <v>31</v>
       </c>
-      <c r="G26" s="178"/>
+      <c r="G26" s="156"/>
       <c r="H26" s="129" t="s">
         <v>33</v>
       </c>
-      <c r="O26" s="179" t="s">
+      <c r="O26" s="157" t="s">
         <v>121</v>
       </c>
-      <c r="P26" s="179"/>
-      <c r="Q26" s="181" t="s">
+      <c r="P26" s="157"/>
+      <c r="Q26" s="158" t="s">
         <v>33</v>
       </c>
-      <c r="R26" s="181"/>
+      <c r="R26" s="158"/>
       <c r="AA26" s="127"/>
       <c r="AC26"/>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="F27" s="179" t="s">
+      <c r="F27" s="157" t="s">
         <v>111</v>
       </c>
-      <c r="G27" s="179"/>
+      <c r="G27" s="157"/>
       <c r="H27" s="134" t="s">
         <v>112</v>
       </c>
@@ -13875,16 +13961,18 @@
     <sortCondition ref="C4:C21"/>
   </sortState>
   <mergeCells count="38">
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="AE1:AE3"/>
     <mergeCell ref="AF1:AF3"/>
     <mergeCell ref="E2:F2"/>
@@ -13901,18 +13989,16 @@
     <mergeCell ref="AB1:AB3"/>
     <mergeCell ref="AC1:AC3"/>
     <mergeCell ref="AD1:AD3"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="U2:V2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13920,10 +14006,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1EE897-404D-4ADC-856A-1E864FE4E3AA}">
-  <dimension ref="A1:AF27"/>
+  <dimension ref="A1:AF25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AK15" sqref="AK15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13963,140 +14049,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" s="1" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="176" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="162" t="s">
+      <c r="B1" s="177"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="185" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="151" t="s">
+      <c r="E1" s="167" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="152"/>
-      <c r="G1" s="151" t="s">
+      <c r="F1" s="168"/>
+      <c r="G1" s="167" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="152"/>
-      <c r="I1" s="151" t="s">
+      <c r="H1" s="168"/>
+      <c r="I1" s="167" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="152"/>
-      <c r="K1" s="151" t="s">
+      <c r="J1" s="168"/>
+      <c r="K1" s="167" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="152"/>
-      <c r="M1" s="151" t="s">
+      <c r="L1" s="168"/>
+      <c r="M1" s="167" t="s">
         <v>87</v>
       </c>
-      <c r="N1" s="152"/>
-      <c r="O1" s="151" t="s">
+      <c r="N1" s="168"/>
+      <c r="O1" s="167" t="s">
         <v>101</v>
       </c>
-      <c r="P1" s="152"/>
-      <c r="Q1" s="151" t="s">
+      <c r="P1" s="168"/>
+      <c r="Q1" s="167" t="s">
         <v>106</v>
       </c>
-      <c r="R1" s="152"/>
-      <c r="S1" s="151" t="s">
+      <c r="R1" s="168"/>
+      <c r="S1" s="167" t="s">
         <v>110</v>
       </c>
-      <c r="T1" s="152"/>
-      <c r="U1" s="151" t="s">
+      <c r="T1" s="168"/>
+      <c r="U1" s="167" t="s">
         <v>114</v>
       </c>
-      <c r="V1" s="152"/>
-      <c r="W1" s="151" t="s">
+      <c r="V1" s="168"/>
+      <c r="W1" s="167" t="s">
         <v>117</v>
       </c>
-      <c r="X1" s="152"/>
-      <c r="Y1" s="151" t="s">
+      <c r="X1" s="168"/>
+      <c r="Y1" s="167" t="s">
         <v>118</v>
       </c>
-      <c r="Z1" s="152"/>
-      <c r="AA1" s="171" t="s">
+      <c r="Z1" s="168"/>
+      <c r="AA1" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="AB1" s="175" t="s">
+      <c r="AB1" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="AC1" s="192" t="s">
+      <c r="AC1" s="187" t="s">
         <v>124</v>
       </c>
-      <c r="AD1" s="193"/>
-      <c r="AE1" s="193"/>
-      <c r="AF1" s="194"/>
+      <c r="AD1" s="188"/>
+      <c r="AE1" s="188"/>
+      <c r="AF1" s="189"/>
     </row>
     <row r="2" spans="1:32" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="155"/>
-      <c r="B2" s="156"/>
-      <c r="C2" s="160"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="169">
+      <c r="A2" s="178"/>
+      <c r="B2" s="179"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="159">
         <v>45418</v>
       </c>
-      <c r="F2" s="170"/>
-      <c r="G2" s="169">
+      <c r="F2" s="160"/>
+      <c r="G2" s="159">
         <v>45425</v>
       </c>
-      <c r="H2" s="170"/>
-      <c r="I2" s="169">
+      <c r="H2" s="160"/>
+      <c r="I2" s="159">
         <v>45432</v>
       </c>
-      <c r="J2" s="170"/>
-      <c r="K2" s="169">
+      <c r="J2" s="160"/>
+      <c r="K2" s="159">
         <v>45439</v>
       </c>
-      <c r="L2" s="170"/>
-      <c r="M2" s="169">
+      <c r="L2" s="160"/>
+      <c r="M2" s="159">
         <v>45446</v>
       </c>
-      <c r="N2" s="170"/>
-      <c r="O2" s="169">
+      <c r="N2" s="160"/>
+      <c r="O2" s="159">
         <v>45453</v>
       </c>
-      <c r="P2" s="170"/>
-      <c r="Q2" s="169">
+      <c r="P2" s="160"/>
+      <c r="Q2" s="159">
         <v>45460</v>
       </c>
-      <c r="R2" s="170"/>
-      <c r="S2" s="169">
+      <c r="R2" s="160"/>
+      <c r="S2" s="159">
         <v>45467</v>
       </c>
-      <c r="T2" s="170"/>
-      <c r="U2" s="169">
+      <c r="T2" s="160"/>
+      <c r="U2" s="159">
         <v>45474</v>
       </c>
-      <c r="V2" s="170"/>
-      <c r="W2" s="169">
+      <c r="V2" s="160"/>
+      <c r="W2" s="159">
         <v>45481</v>
       </c>
-      <c r="X2" s="170"/>
-      <c r="Y2" s="169">
+      <c r="X2" s="160"/>
+      <c r="Y2" s="159">
         <v>45488</v>
       </c>
-      <c r="Z2" s="170"/>
-      <c r="AA2" s="172"/>
-      <c r="AB2" s="190"/>
-      <c r="AC2" s="195" t="s">
+      <c r="Z2" s="160"/>
+      <c r="AA2" s="170"/>
+      <c r="AB2" s="192"/>
+      <c r="AC2" s="190" t="s">
         <v>105</v>
       </c>
-      <c r="AD2" s="164" t="s">
+      <c r="AD2" s="162" t="s">
         <v>123</v>
       </c>
-      <c r="AE2" s="164" t="s">
+      <c r="AE2" s="162" t="s">
         <v>48</v>
       </c>
-      <c r="AF2" s="164" t="s">
+      <c r="AF2" s="162" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:32" s="1" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="157"/>
-      <c r="B3" s="158"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="163"/>
+      <c r="A3" s="180"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="184"/>
+      <c r="D3" s="186"/>
       <c r="E3" s="61" t="s">
         <v>28</v>
       </c>
@@ -14163,12 +14249,12 @@
       <c r="Z3" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="AA3" s="173"/>
-      <c r="AB3" s="191"/>
-      <c r="AC3" s="196"/>
-      <c r="AD3" s="166"/>
-      <c r="AE3" s="166"/>
-      <c r="AF3" s="166"/>
+      <c r="AA3" s="171"/>
+      <c r="AB3" s="193"/>
+      <c r="AC3" s="191"/>
+      <c r="AD3" s="164"/>
+      <c r="AE3" s="164"/>
+      <c r="AF3" s="164"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
@@ -14231,25 +14317,25 @@
       <c r="Y4" s="147"/>
       <c r="Z4" s="139"/>
       <c r="AA4" s="73">
-        <f t="shared" ref="AA4:AA19" si="0">SUMIF(E4:Y4,"&gt;30")</f>
+        <f>SUMIF(E4:Y4,"&gt;30")</f>
         <v>278</v>
       </c>
       <c r="AB4" s="74">
         <f>AA4/AC4</f>
         <v>46.333333333333336</v>
       </c>
-      <c r="AC4" s="186">
-        <f t="shared" ref="AC4:AC19" si="1">COUNTIF(E4:Y4,"&gt;30")</f>
-        <v>6</v>
-      </c>
-      <c r="AD4" s="187">
-        <v>2</v>
-      </c>
-      <c r="AE4" s="188">
+      <c r="AC4" s="149">
+        <f>COUNTIF(E4:Y4,"&gt;30")</f>
+        <v>6</v>
+      </c>
+      <c r="AD4" s="150">
+        <v>2</v>
+      </c>
+      <c r="AE4" s="151">
         <f>SUMIF(E4:Z4,"&lt;30")+AD4</f>
         <v>115</v>
       </c>
-      <c r="AF4" s="189">
+      <c r="AF4" s="152">
         <f>(AE4)/AC4</f>
         <v>19.166666666666668</v>
       </c>
@@ -14331,7 +14417,7 @@
         <v>20</v>
       </c>
       <c r="AA5" s="73">
-        <f t="shared" si="0"/>
+        <f>SUMIF(E5:Y5,"&gt;30")</f>
         <v>501</v>
       </c>
       <c r="AB5" s="74">
@@ -14339,7 +14425,7 @@
         <v>50.1</v>
       </c>
       <c r="AC5" s="130">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(E5:Y5,"&gt;30")</f>
         <v>10</v>
       </c>
       <c r="AD5" s="89">
@@ -14433,7 +14519,7 @@
         <v>18</v>
       </c>
       <c r="AA6" s="73">
-        <f t="shared" si="0"/>
+        <f>SUMIF(E6:Y6,"&gt;30")</f>
         <v>399</v>
       </c>
       <c r="AB6" s="74">
@@ -14441,7 +14527,7 @@
         <v>44.333333333333336</v>
       </c>
       <c r="AC6" s="130">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(E6:Y6,"&gt;30")</f>
         <v>9</v>
       </c>
       <c r="AD6" s="89">
@@ -14537,7 +14623,7 @@
         <v>20</v>
       </c>
       <c r="AA7" s="73">
-        <f t="shared" si="0"/>
+        <f>SUMIF(E7:Y7,"&gt;30")</f>
         <v>537</v>
       </c>
       <c r="AB7" s="74">
@@ -14545,7 +14631,7 @@
         <v>48.81818181818182</v>
       </c>
       <c r="AC7" s="130">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(E7:Y7,"&gt;30")</f>
         <v>11</v>
       </c>
       <c r="AD7" s="89">
@@ -14633,7 +14719,7 @@
         <v>18</v>
       </c>
       <c r="AA8" s="73">
-        <f t="shared" si="0"/>
+        <f>SUMIF(E8:Y8,"&gt;30")</f>
         <v>515</v>
       </c>
       <c r="AB8" s="74">
@@ -14641,7 +14727,7 @@
         <v>57.222222222222221</v>
       </c>
       <c r="AC8" s="130">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(E8:Y8,"&gt;30")</f>
         <v>9</v>
       </c>
       <c r="AD8" s="89">
@@ -14729,7 +14815,7 @@
       <c r="Y9" s="86"/>
       <c r="Z9" s="84"/>
       <c r="AA9" s="73">
-        <f t="shared" si="0"/>
+        <f>SUMIF(E9:Y9,"&gt;30")</f>
         <v>465</v>
       </c>
       <c r="AB9" s="74">
@@ -14737,7 +14823,7 @@
         <v>51.666666666666664</v>
       </c>
       <c r="AC9" s="130">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(E9:Y9,"&gt;30")</f>
         <v>9</v>
       </c>
       <c r="AD9" s="89">
@@ -14821,7 +14907,7 @@
         <v>19</v>
       </c>
       <c r="AA10" s="73">
-        <f t="shared" si="0"/>
+        <f>SUMIF(E10:Y10,"&gt;30")</f>
         <v>417</v>
       </c>
       <c r="AB10" s="74">
@@ -14829,7 +14915,7 @@
         <v>52.125</v>
       </c>
       <c r="AC10" s="130">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(E10:Y10,"&gt;30")</f>
         <v>8</v>
       </c>
       <c r="AD10" s="89">
@@ -14909,7 +14995,7 @@
       <c r="Y11" s="86"/>
       <c r="Z11" s="84"/>
       <c r="AA11" s="73">
-        <f t="shared" si="0"/>
+        <f>SUMIF(E11:Y11,"&gt;30")</f>
         <v>266</v>
       </c>
       <c r="AB11" s="74">
@@ -14917,7 +15003,7 @@
         <v>38</v>
       </c>
       <c r="AC11" s="130">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(E11:Y11,"&gt;30")</f>
         <v>7</v>
       </c>
       <c r="AD11" s="89">
@@ -14997,7 +15083,7 @@
       <c r="Y12" s="86"/>
       <c r="Z12" s="84"/>
       <c r="AA12" s="73">
-        <f t="shared" si="0"/>
+        <f>SUMIF(E12:Y12,"&gt;30")</f>
         <v>339</v>
       </c>
       <c r="AB12" s="74">
@@ -15005,7 +15091,7 @@
         <v>48.428571428571431</v>
       </c>
       <c r="AC12" s="130">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(E12:Y12,"&gt;30")</f>
         <v>7</v>
       </c>
       <c r="AD12" s="89">
@@ -15085,15 +15171,15 @@
         <v>17</v>
       </c>
       <c r="AA13" s="73">
-        <f t="shared" si="0"/>
+        <f>SUMIF(E13:Y13,"&gt;30")</f>
         <v>316</v>
       </c>
       <c r="AB13" s="74">
         <f>AA13/AC13</f>
         <v>45.142857142857146</v>
       </c>
-      <c r="AC13" s="130">
-        <f t="shared" si="1"/>
+      <c r="AC13" s="199">
+        <f>COUNTIF(E13:Y13,"&gt;30")</f>
         <v>7</v>
       </c>
       <c r="AD13" s="89">
@@ -15110,242 +15196,242 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="77" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B14" s="78" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14" s="79" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="80">
         <f>ROUND(AB14-36,2)</f>
-        <v>18.25</v>
+        <v>21.5</v>
       </c>
       <c r="E14" s="81">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F14" s="82">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G14" s="81">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H14" s="82">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I14" s="83"/>
       <c r="J14" s="84"/>
       <c r="K14" s="86"/>
       <c r="L14" s="84"/>
       <c r="M14" s="92">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="N14" s="88">
-        <v>15</v>
-      </c>
-      <c r="O14" s="92">
+        <v>13</v>
+      </c>
+      <c r="O14" s="98">
         <v>54</v>
       </c>
       <c r="P14" s="88">
-        <v>19</v>
-      </c>
-      <c r="Q14" s="86"/>
-      <c r="R14" s="84"/>
+        <v>21</v>
+      </c>
+      <c r="Q14" s="87">
+        <v>61</v>
+      </c>
+      <c r="R14" s="88">
+        <v>13</v>
+      </c>
       <c r="S14" s="86"/>
       <c r="T14" s="84"/>
-      <c r="U14" s="86"/>
-      <c r="V14" s="84"/>
+      <c r="U14" s="95">
+        <v>61</v>
+      </c>
+      <c r="V14" s="82">
+        <v>14</v>
+      </c>
       <c r="W14" s="86"/>
       <c r="X14" s="84"/>
       <c r="Y14" s="86"/>
       <c r="Z14" s="84"/>
       <c r="AA14" s="73">
-        <f t="shared" si="0"/>
-        <v>217</v>
+        <f>SUMIF(E14:Y14,"&gt;30")</f>
+        <v>345</v>
       </c>
       <c r="AB14" s="74">
         <f>AA14/AC14</f>
-        <v>54.25</v>
+        <v>57.5</v>
       </c>
       <c r="AC14" s="130">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f>COUNTIF(E14:Y14,"&gt;30")</f>
+        <v>6</v>
       </c>
       <c r="AD14" s="89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE14" s="76">
         <f>SUMIF(E14:Z14,"&lt;30")+AD14</f>
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="AF14" s="90">
         <f>(AE14)/AC14</f>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="77" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B15" s="78" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C15" s="79" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D15" s="80">
         <f>ROUND(AB15-36,2)</f>
-        <v>15</v>
-      </c>
-      <c r="E15" s="83"/>
-      <c r="F15" s="84"/>
+        <v>18.25</v>
+      </c>
+      <c r="E15" s="81">
+        <v>52</v>
+      </c>
+      <c r="F15" s="82">
+        <v>20</v>
+      </c>
       <c r="G15" s="81">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="H15" s="82">
-        <v>20</v>
-      </c>
-      <c r="I15" s="81">
-        <v>47</v>
-      </c>
-      <c r="J15" s="82">
-        <v>21</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I15" s="83"/>
+      <c r="J15" s="84"/>
       <c r="K15" s="86"/>
       <c r="L15" s="84"/>
       <c r="M15" s="92">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N15" s="88">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="O15" s="92">
         <v>54</v>
       </c>
       <c r="P15" s="88">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="Q15" s="86"/>
       <c r="R15" s="84"/>
       <c r="S15" s="86"/>
       <c r="T15" s="84"/>
-      <c r="U15" s="95">
-        <v>50</v>
-      </c>
-      <c r="V15" s="82">
-        <v>19</v>
-      </c>
+      <c r="U15" s="86"/>
+      <c r="V15" s="84"/>
       <c r="W15" s="86"/>
       <c r="X15" s="84"/>
       <c r="Y15" s="86"/>
       <c r="Z15" s="84"/>
       <c r="AA15" s="73">
-        <f t="shared" si="0"/>
-        <v>255</v>
+        <f>SUMIF(E15:Y15,"&gt;30")</f>
+        <v>217</v>
       </c>
       <c r="AB15" s="74">
         <f>AA15/AC15</f>
-        <v>51</v>
-      </c>
-      <c r="AC15" s="130">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <v>54.25</v>
+      </c>
+      <c r="AC15" s="200">
+        <f>COUNTIF(E15:Y15,"&gt;30")</f>
+        <v>4</v>
       </c>
       <c r="AD15" s="89">
         <v>0</v>
       </c>
       <c r="AE15" s="76">
         <f>SUMIF(E15:Z15,"&lt;30")+AD15</f>
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="AF15" s="90">
         <f>(AE15)/AC15</f>
-        <v>17.600000000000001</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="77" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B16" s="78" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C16" s="79" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D16" s="80">
         <f>ROUND(AB16-36,2)</f>
-        <v>21.5</v>
-      </c>
-      <c r="E16" s="81">
-        <v>53</v>
-      </c>
-      <c r="F16" s="82">
+        <v>15</v>
+      </c>
+      <c r="E16" s="83"/>
+      <c r="F16" s="84"/>
+      <c r="G16" s="81">
+        <v>48</v>
+      </c>
+      <c r="H16" s="82">
+        <v>20</v>
+      </c>
+      <c r="I16" s="81">
+        <v>47</v>
+      </c>
+      <c r="J16" s="82">
         <v>21</v>
       </c>
-      <c r="G16" s="81">
-        <v>55</v>
-      </c>
-      <c r="H16" s="82">
-        <v>19</v>
-      </c>
-      <c r="I16" s="83"/>
-      <c r="J16" s="84"/>
       <c r="K16" s="86"/>
       <c r="L16" s="84"/>
       <c r="M16" s="99">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N16" s="100">
-        <v>13</v>
-      </c>
-      <c r="O16" s="98">
+        <v>12</v>
+      </c>
+      <c r="O16" s="92">
         <v>54</v>
       </c>
       <c r="P16" s="88">
-        <v>21</v>
-      </c>
-      <c r="Q16" s="87">
-        <v>61</v>
-      </c>
-      <c r="R16" s="88">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="Q16" s="86"/>
+      <c r="R16" s="84"/>
       <c r="S16" s="86"/>
       <c r="T16" s="84"/>
       <c r="U16" s="95">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="V16" s="82">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="W16" s="86"/>
       <c r="X16" s="84"/>
       <c r="Y16" s="86"/>
       <c r="Z16" s="84"/>
       <c r="AA16" s="73">
-        <f t="shared" si="0"/>
-        <v>345</v>
+        <f>SUMIF(E16:Y16,"&gt;30")</f>
+        <v>255</v>
       </c>
       <c r="AB16" s="74">
         <f>AA16/AC16</f>
-        <v>57.5</v>
-      </c>
-      <c r="AC16" s="130">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <v>51</v>
+      </c>
+      <c r="AC16" s="200">
+        <f>COUNTIF(E16:Y16,"&gt;30")</f>
+        <v>5</v>
       </c>
       <c r="AD16" s="89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE16" s="76">
         <f>SUMIF(E16:Z16,"&lt;30")+AD16</f>
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="AF16" s="90">
         <f>(AE16)/AC16</f>
-        <v>17</v>
+        <v>17.600000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
@@ -15388,15 +15474,15 @@
       <c r="Y17" s="86"/>
       <c r="Z17" s="84"/>
       <c r="AA17" s="73">
-        <f t="shared" si="0"/>
+        <f>SUMIF(E17:Y17,"&gt;30")</f>
         <v>52</v>
       </c>
       <c r="AB17" s="74">
         <f>AA17/AC17</f>
         <v>52</v>
       </c>
-      <c r="AC17" s="130">
-        <f t="shared" si="1"/>
+      <c r="AC17" s="200">
+        <f>COUNTIF(E17:Y17,"&gt;30")</f>
         <v>1</v>
       </c>
       <c r="AD17" s="76">
@@ -15451,15 +15537,15 @@
       <c r="Y18" s="101"/>
       <c r="Z18" s="102"/>
       <c r="AA18" s="73">
-        <f t="shared" si="0"/>
+        <f>SUMIF(E18:Y18,"&gt;30")</f>
         <v>64</v>
       </c>
       <c r="AB18" s="74">
         <f>AA18/AC18</f>
         <v>64</v>
       </c>
-      <c r="AC18" s="130">
-        <f t="shared" si="1"/>
+      <c r="AC18" s="200">
+        <f>COUNTIF(E18:Y18,"&gt;30")</f>
         <v>1</v>
       </c>
       <c r="AD18" s="89">
@@ -15474,296 +15560,200 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A19" s="103" t="s">
+    <row r="19" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="114" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="104" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="105" t="s">
+      <c r="B19" s="115" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="116" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="80" t="s">
+      <c r="D19" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="106"/>
-      <c r="F19" s="102"/>
-      <c r="G19" s="106"/>
-      <c r="H19" s="102"/>
-      <c r="I19" s="106"/>
-      <c r="J19" s="102"/>
-      <c r="K19" s="135">
+      <c r="E19" s="118"/>
+      <c r="F19" s="119"/>
+      <c r="G19" s="118"/>
+      <c r="H19" s="119"/>
+      <c r="I19" s="118"/>
+      <c r="J19" s="119"/>
+      <c r="K19" s="201">
         <v>50</v>
       </c>
-      <c r="L19" s="136">
+      <c r="L19" s="202">
         <v>0</v>
       </c>
-      <c r="M19" s="86"/>
-      <c r="N19" s="84"/>
-      <c r="O19" s="86"/>
-      <c r="P19" s="84"/>
-      <c r="Q19" s="86"/>
-      <c r="R19" s="84"/>
-      <c r="S19" s="86"/>
-      <c r="T19" s="84"/>
-      <c r="U19" s="86"/>
-      <c r="V19" s="84"/>
-      <c r="W19" s="86"/>
-      <c r="X19" s="84"/>
-      <c r="Y19" s="86"/>
-      <c r="Z19" s="84"/>
-      <c r="AA19" s="73">
-        <f t="shared" si="0"/>
+      <c r="M19" s="120"/>
+      <c r="N19" s="119"/>
+      <c r="O19" s="120"/>
+      <c r="P19" s="119"/>
+      <c r="Q19" s="120"/>
+      <c r="R19" s="119"/>
+      <c r="S19" s="120"/>
+      <c r="T19" s="119"/>
+      <c r="U19" s="120"/>
+      <c r="V19" s="119"/>
+      <c r="W19" s="120"/>
+      <c r="X19" s="119"/>
+      <c r="Y19" s="120"/>
+      <c r="Z19" s="119"/>
+      <c r="AA19" s="203">
+        <f>SUMIF(E19:Y19,"&gt;30")</f>
         <v>50</v>
       </c>
-      <c r="AB19" s="74">
+      <c r="AB19" s="204">
         <f>AA19/AC19</f>
         <v>50</v>
       </c>
-      <c r="AC19" s="130">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AD19" s="89">
+      <c r="AC19" s="205">
+        <f>COUNTIF(E19:Y19,"&gt;30")</f>
+        <v>1</v>
+      </c>
+      <c r="AD19" s="206">
         <v>0</v>
       </c>
-      <c r="AE19" s="76">
+      <c r="AE19" s="207">
         <f>SUMIF(E19:Z19,"&lt;30")+AD19</f>
         <v>0</v>
       </c>
-      <c r="AF19" s="90">
+      <c r="AF19" s="208">
         <f>(AE19)/AC19</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A20" s="103" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="105" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="113" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="106"/>
-      <c r="F20" s="102"/>
-      <c r="G20" s="106"/>
-      <c r="H20" s="102"/>
-      <c r="I20" s="106"/>
-      <c r="J20" s="102"/>
-      <c r="K20" s="86"/>
-      <c r="L20" s="84"/>
-      <c r="M20" s="86"/>
-      <c r="N20" s="84"/>
-      <c r="O20" s="86"/>
-      <c r="P20" s="84"/>
-      <c r="Q20" s="86"/>
-      <c r="R20" s="84"/>
-      <c r="S20" s="86"/>
-      <c r="T20" s="84"/>
-      <c r="U20" s="86"/>
-      <c r="V20" s="84"/>
-      <c r="W20" s="86"/>
-      <c r="X20" s="84"/>
-      <c r="Y20" s="86"/>
-      <c r="Z20" s="84"/>
-      <c r="AA20" s="107"/>
-      <c r="AB20" s="109"/>
-      <c r="AC20" s="108"/>
-      <c r="AD20" s="110"/>
-      <c r="AE20" s="111"/>
-      <c r="AF20" s="112"/>
-    </row>
-    <row r="21" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="114" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="115" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="116" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="117" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="118"/>
-      <c r="F21" s="119"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="119"/>
-      <c r="I21" s="118"/>
-      <c r="J21" s="119"/>
-      <c r="K21" s="120"/>
-      <c r="L21" s="119"/>
-      <c r="M21" s="120"/>
-      <c r="N21" s="119"/>
-      <c r="O21" s="120"/>
-      <c r="P21" s="119"/>
-      <c r="Q21" s="120"/>
-      <c r="R21" s="119"/>
-      <c r="S21" s="120"/>
-      <c r="T21" s="119"/>
-      <c r="U21" s="120"/>
-      <c r="V21" s="119"/>
-      <c r="W21" s="120"/>
-      <c r="X21" s="119"/>
-      <c r="Y21" s="120"/>
-      <c r="Z21" s="119"/>
-      <c r="AA21" s="121"/>
-      <c r="AB21" s="123"/>
-      <c r="AC21" s="122"/>
-      <c r="AD21" s="124"/>
-      <c r="AE21" s="125"/>
-      <c r="AF21" s="126"/>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="E22" s="127">
-        <f>AVERAGEIF(E4:E21,"&gt;0")</f>
+      <c r="E20" s="127">
+        <f>AVERAGEIF(E4:E19,"&gt;0")</f>
         <v>50.090909090909093</v>
       </c>
-      <c r="F22" s="127"/>
-      <c r="G22" s="127">
-        <f>AVERAGEIF(G4:G21,"&gt;0")</f>
+      <c r="F20" s="127"/>
+      <c r="G20" s="127">
+        <f>AVERAGEIF(G4:G19,"&gt;0")</f>
         <v>48.583333333333336</v>
       </c>
-      <c r="H22" s="127"/>
-      <c r="I22" s="127">
-        <f>AVERAGEIF(I4:I21,"&gt;0")</f>
+      <c r="H20" s="127"/>
+      <c r="I20" s="127">
+        <f>AVERAGEIF(I4:I19,"&gt;0")</f>
         <v>49.777777777777779</v>
       </c>
-      <c r="J22" s="127"/>
-      <c r="K22" s="127">
-        <f>AVERAGEIF(K4:K21,"&gt;0")</f>
+      <c r="J20" s="127"/>
+      <c r="K20" s="127">
+        <f>AVERAGEIF(K4:K19,"&gt;0")</f>
         <v>49.875</v>
       </c>
-      <c r="L22" s="127"/>
-      <c r="M22" s="127">
-        <f>AVERAGEIF(M4:M21,"&gt;0")</f>
+      <c r="L20" s="127"/>
+      <c r="M20" s="127">
+        <f>AVERAGEIF(M4:M19,"&gt;0")</f>
         <v>51.636363636363633</v>
       </c>
-      <c r="N22" s="127"/>
-      <c r="O22" s="127">
-        <f>AVERAGEIF(O4:O21,"&gt;0")</f>
+      <c r="N20" s="127"/>
+      <c r="O20" s="127">
+        <f>AVERAGEIF(O4:O19,"&gt;0")</f>
         <v>49.5</v>
       </c>
-      <c r="P22" s="127"/>
-      <c r="Q22" s="127">
-        <f>AVERAGEIF(Q4:Q21,"&gt;0")</f>
+      <c r="P20" s="127"/>
+      <c r="Q20" s="127">
+        <f>AVERAGEIF(Q4:Q19,"&gt;0")</f>
         <v>50.428571428571431</v>
       </c>
-      <c r="R22" s="127"/>
-      <c r="S22" s="127">
-        <f>AVERAGEIF(S4:S21,"&gt;0")</f>
+      <c r="R20" s="127"/>
+      <c r="S20" s="127">
+        <f>AVERAGEIF(S4:S19,"&gt;0")</f>
         <v>47.714285714285715</v>
       </c>
-      <c r="T22" s="127"/>
-      <c r="U22" s="127">
-        <f>AVERAGEIF(U4:U21,"&gt;0")</f>
+      <c r="T20" s="127"/>
+      <c r="U20" s="127">
+        <f>AVERAGEIF(U4:U19,"&gt;0")</f>
         <v>50.727272727272727</v>
       </c>
-      <c r="V22" s="127"/>
-      <c r="W22" s="127">
-        <f>AVERAGEIF(W4:W21,"&gt;0")</f>
+      <c r="V20" s="127"/>
+      <c r="W20" s="127">
+        <f>AVERAGEIF(W4:W19,"&gt;0")</f>
         <v>48</v>
       </c>
-      <c r="X22" s="127"/>
-      <c r="Y22" s="127">
-        <f>AVERAGEIF(Y4:Y21,"&gt;0")</f>
+      <c r="X20" s="127"/>
+      <c r="Y20" s="127">
+        <f>AVERAGEIF(Y4:Y19,"&gt;0")</f>
         <v>48.666666666666664</v>
       </c>
-      <c r="Z22" s="127"/>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="D24" s="178" t="s">
+      <c r="Z20" s="127"/>
+    </row>
+    <row r="22" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="156" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="178"/>
-      <c r="F24" s="128" t="s">
+      <c r="E22" s="156"/>
+      <c r="F22" s="128" t="s">
         <v>32</v>
       </c>
-      <c r="W24" s="185" t="s">
+      <c r="W22" s="148" t="s">
         <v>32</v>
+      </c>
+      <c r="AA22" s="127"/>
+      <c r="AB22"/>
+    </row>
+    <row r="23" spans="1:32" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="156" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="156"/>
+      <c r="F23" s="129" t="s">
+        <v>33</v>
+      </c>
+      <c r="R23" s="143"/>
+      <c r="U23" s="156" t="s">
+        <v>30</v>
+      </c>
+      <c r="V23" s="156"/>
+      <c r="W23" s="129" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y23" s="197"/>
+      <c r="Z23" s="198" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA23" s="198"/>
+      <c r="AB23" s="198"/>
+    </row>
+    <row r="24" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="157" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" s="157"/>
+      <c r="F24" s="134" t="s">
+        <v>112</v>
+      </c>
+      <c r="R24" s="144"/>
+      <c r="U24" s="156" t="s">
+        <v>31</v>
+      </c>
+      <c r="V24" s="156"/>
+      <c r="W24" s="134" t="s">
+        <v>112</v>
       </c>
       <c r="AA24" s="127"/>
       <c r="AB24"/>
     </row>
-    <row r="25" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="178" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" s="178"/>
-      <c r="F25" s="129" t="s">
-        <v>33</v>
-      </c>
-      <c r="R25" s="143"/>
-      <c r="U25" s="178" t="s">
-        <v>30</v>
-      </c>
-      <c r="V25" s="178"/>
-      <c r="W25" s="129" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA25" s="127"/>
-      <c r="AB25"/>
-    </row>
-    <row r="26" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="59"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="179" t="s">
-        <v>122</v>
-      </c>
-      <c r="E26" s="179"/>
-      <c r="F26" s="134" t="s">
-        <v>112</v>
-      </c>
-      <c r="R26" s="144"/>
-      <c r="U26" s="178" t="s">
-        <v>31</v>
-      </c>
-      <c r="V26" s="178"/>
-      <c r="W26" s="134" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA26" s="127"/>
-      <c r="AB26"/>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="U27" s="179" t="s">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="U25" s="157" t="s">
         <v>111</v>
       </c>
-      <c r="V27" s="179"/>
-      <c r="W27" s="134"/>
+      <c r="V25" s="157"/>
+      <c r="W25" s="134"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:AF21">
-    <sortCondition descending="1" ref="AF4:AF21"/>
-    <sortCondition ref="C4:C21"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:AF19">
+    <sortCondition descending="1" sortBy="cellColor" ref="AC4:AC19" dxfId="1"/>
+    <sortCondition descending="1" ref="AF4:AF19"/>
+    <sortCondition ref="C4:C19"/>
   </sortState>
   <mergeCells count="38">
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="U25:V25"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="S2:T2"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="Y1:Z1"/>
@@ -15772,8 +15762,14 @@
     <mergeCell ref="AC2:AC3"/>
     <mergeCell ref="AD2:AD3"/>
     <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="AA1:AA3"/>
+    <mergeCell ref="AB1:AB3"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="S2:T2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
@@ -15781,10 +15777,21 @@
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="O1:P1"/>
-    <mergeCell ref="AA1:AA3"/>
-    <mergeCell ref="AB1:AB3"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="U2:V2"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="U25:V25"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -17423,23 +17430,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="153" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="149"/>
-      <c r="J1" s="149"/>
-      <c r="K1" s="149"/>
-      <c r="L1" s="149"/>
-      <c r="M1" s="149"/>
-      <c r="N1" s="149"/>
-      <c r="O1" s="149"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="154"/>
+      <c r="O1" s="154"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -17453,23 +17460,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="155" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="149"/>
-      <c r="L2" s="149"/>
-      <c r="M2" s="149"/>
-      <c r="N2" s="149"/>
-      <c r="O2" s="149"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="154"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="154"/>
+      <c r="O2" s="154"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -18995,23 +19002,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="153" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="149"/>
-      <c r="J1" s="149"/>
-      <c r="K1" s="149"/>
-      <c r="L1" s="149"/>
-      <c r="M1" s="149"/>
-      <c r="N1" s="149"/>
-      <c r="O1" s="149"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="154"/>
+      <c r="O1" s="154"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -19025,23 +19032,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="155" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="149"/>
-      <c r="L2" s="149"/>
-      <c r="M2" s="149"/>
-      <c r="N2" s="149"/>
-      <c r="O2" s="149"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="154"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="154"/>
+      <c r="O2" s="154"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -20656,23 +20663,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="153" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="149"/>
-      <c r="J1" s="149"/>
-      <c r="K1" s="149"/>
-      <c r="L1" s="149"/>
-      <c r="M1" s="149"/>
-      <c r="N1" s="149"/>
-      <c r="O1" s="149"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="154"/>
+      <c r="O1" s="154"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -20686,23 +20693,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="155" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="149"/>
-      <c r="L2" s="149"/>
-      <c r="M2" s="149"/>
-      <c r="N2" s="149"/>
-      <c r="O2" s="149"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="154"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="154"/>
+      <c r="O2" s="154"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -22108,23 +22115,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="153" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="149"/>
-      <c r="J1" s="149"/>
-      <c r="K1" s="149"/>
-      <c r="L1" s="149"/>
-      <c r="M1" s="149"/>
-      <c r="N1" s="149"/>
-      <c r="O1" s="149"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="154"/>
+      <c r="O1" s="154"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -22138,23 +22145,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="155" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="149"/>
-      <c r="L2" s="149"/>
-      <c r="M2" s="149"/>
-      <c r="N2" s="149"/>
-      <c r="O2" s="149"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="154"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="154"/>
+      <c r="O2" s="154"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>

</xml_diff>